<commit_message>
Update script - type_a/type_b
</commit_message>
<xml_diff>
--- a/output/Block_Master.xlsx
+++ b/output/Block_Master.xlsx
@@ -32,9 +32,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -65,8 +66,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,145 +406,145 @@
   </sheetViews>
   <sheetData>
     <row r="1">
-      <c r="A1" t="str">
+      <c r="A1" s="1" t="str">
         <v>Block Name</v>
       </c>
-      <c r="B1" t="str">
+      <c r="B1" s="1" t="str">
         <v>State</v>
       </c>
-      <c r="C1" t="str">
+      <c r="C1" s="1" t="str">
         <v>District</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="str">
+      <c r="A2" s="1" t="str">
         <v>Karimpur I</v>
       </c>
-      <c r="B2" t="str">
-        <v>West Bengal</v>
-      </c>
-      <c r="C2" t="str">
+      <c r="B2" s="1" t="str">
+        <v>West Bengal</v>
+      </c>
+      <c r="C2" s="1" t="str">
         <v>Nadia</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="str">
+      <c r="A3" s="1" t="str">
         <v>Karimpur II</v>
       </c>
-      <c r="B3" t="str">
-        <v>West Bengal</v>
-      </c>
-      <c r="C3" t="str">
+      <c r="B3" s="1" t="str">
+        <v>West Bengal</v>
+      </c>
+      <c r="C3" s="1" t="str">
         <v>Nadia</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="str">
+      <c r="A4" s="1" t="str">
         <v>Chapra</v>
       </c>
-      <c r="B4" t="str">
-        <v>West Bengal</v>
-      </c>
-      <c r="C4" t="str">
+      <c r="B4" s="1" t="str">
+        <v>West Bengal</v>
+      </c>
+      <c r="C4" s="1" t="str">
         <v>Nadia</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="str">
+      <c r="A5" s="1" t="str">
         <v>Tehatta I</v>
       </c>
-      <c r="B5" t="str">
-        <v>West Bengal</v>
-      </c>
-      <c r="C5" t="str">
+      <c r="B5" s="1" t="str">
+        <v>West Bengal</v>
+      </c>
+      <c r="C5" s="1" t="str">
         <v>Nadia</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="str">
+      <c r="A6" s="1" t="str">
         <v>Tehatta II</v>
       </c>
-      <c r="B6" t="str">
-        <v>West Bengal</v>
-      </c>
-      <c r="C6" t="str">
+      <c r="B6" s="1" t="str">
+        <v>West Bengal</v>
+      </c>
+      <c r="C6" s="1" t="str">
         <v>Nadia</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="str">
+      <c r="A7" s="1" t="str">
         <v>Hanskhali</v>
       </c>
-      <c r="B7" t="str">
-        <v>West Bengal</v>
-      </c>
-      <c r="C7" t="str">
+      <c r="B7" s="1" t="str">
+        <v>West Bengal</v>
+      </c>
+      <c r="C7" s="1" t="str">
         <v>Nadia</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="str">
+      <c r="A8" s="1" t="str">
         <v>Nabadwip</v>
       </c>
-      <c r="B8" t="str">
-        <v>West Bengal</v>
-      </c>
-      <c r="C8" t="str">
+      <c r="B8" s="1" t="str">
+        <v>West Bengal</v>
+      </c>
+      <c r="C8" s="1" t="str">
         <v>Nadia</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="str">
+      <c r="A9" s="1" t="str">
         <v>Ranaghat I</v>
       </c>
-      <c r="B9" t="str">
-        <v>West Bengal</v>
-      </c>
-      <c r="C9" t="str">
+      <c r="B9" s="1" t="str">
+        <v>West Bengal</v>
+      </c>
+      <c r="C9" s="1" t="str">
         <v>Nadia</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="str">
+      <c r="A10" s="1" t="str">
         <v>Ranaghat II</v>
       </c>
-      <c r="B10" t="str">
-        <v>West Bengal</v>
-      </c>
-      <c r="C10" t="str">
+      <c r="B10" s="1" t="str">
+        <v>West Bengal</v>
+      </c>
+      <c r="C10" s="1" t="str">
         <v>Nadia</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="str">
+      <c r="A11" s="1" t="str">
         <v>Shantipur</v>
       </c>
-      <c r="B11" t="str">
-        <v>West Bengal</v>
-      </c>
-      <c r="C11" t="str">
+      <c r="B11" s="1" t="str">
+        <v>West Bengal</v>
+      </c>
+      <c r="C11" s="1" t="str">
         <v>Nadia</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="str">
+      <c r="A12" s="1" t="str">
         <v>Krishnagar I</v>
       </c>
-      <c r="B12" t="str">
-        <v>West Bengal</v>
-      </c>
-      <c r="C12" t="str">
+      <c r="B12" s="1" t="str">
+        <v>West Bengal</v>
+      </c>
+      <c r="C12" s="1" t="str">
         <v>Nadia</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="str">
+      <c r="A13" s="1" t="str">
         <v>Krishnaganj</v>
       </c>
-      <c r="B13" t="str">
-        <v>West Bengal</v>
-      </c>
-      <c r="C13" t="str">
+      <c r="B13" s="1" t="str">
+        <v>West Bengal</v>
+      </c>
+      <c r="C13" s="1" t="str">
         <v>Nadia</v>
       </c>
     </row>

</xml_diff>